<commit_message>
Update Bending and Barrowman Calcs.xlsx
</commit_message>
<xml_diff>
--- a/Bending and Barrowman Calcs.xlsx
+++ b/Bending and Barrowman Calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kchee\OneDrive\Documents\Clubs and Fun\APRL Github\Vehicle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90395CF6-EE17-4774-8B63-EAE2167E0043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F40A86-A0A0-4D92-86F2-356278A032A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89B1A080-25E0-4FFB-AE02-629D748CE398}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{89B1A080-25E0-4FFB-AE02-629D748CE398}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1729,6 +1729,50 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>419786</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4758A6D4-EF0E-6390-C267-77DB42FB5F62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26517600" y="895350"/>
+          <a:ext cx="4915586" cy="8249801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2051,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A825FAF-4742-4B1C-8FEE-CCCA86FED367}">
   <dimension ref="A1:AD83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O2" workbookViewId="0">
-      <selection activeCell="AN17" sqref="AN17"/>
+    <sheetView tabSelected="1" topLeftCell="AH4" workbookViewId="0">
+      <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>